<commit_message>
Slides and Spreadsheets for VaR for Bonds up
</commit_message>
<xml_diff>
--- a/lectures/3Bonds/Spreadsheets/3.1 Bond Valuation Example.xlsx
+++ b/lectures/3Bonds/Spreadsheets/3.1 Bond Valuation Example.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcfma\Documents\GitHub\math100_2\lectures\3Bonds\Other Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fefe2130b16d0f35/0 Bago/1 Math Dept/_SY 21-22 1st Sem/MATH 100.2/Lectures/1 Review of Fixed-Income Securities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22988EE7-A337-48FA-BC2B-F950388FDAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{14BB454B-57D7-451A-962C-BF53979E4108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42E54DDE-0EEA-4B56-9E05-EEB583C86DE1}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{70B22532-65DC-4636-8A51-430209A39212}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
+    <sheet name="Answer" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Coupon Dates</t>
   </si>
@@ -84,12 +85,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -110,12 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +441,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2">
-        <f ca="1">TODAY()</f>
+        <f ca="1">TODAY()-2</f>
         <v>44481</v>
       </c>
     </row>
@@ -478,22 +486,187 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>44561</v>
+        <v>44545</v>
       </c>
       <c r="B5">
         <f ca="1">(A5-$B$1)/360</f>
-        <v>0.22222222222222221</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
       <c r="D5">
         <f ca="1">EXP(-$B$2*B5)</f>
-        <v>0.9758519014070135</v>
+        <v>0.98063441398564755</v>
       </c>
       <c r="E5">
         <f ca="1">C5*D5</f>
-        <v>97.585190140701343</v>
+        <v>98.063441398564748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f>DATE(YEAR(A5)+1,MONTH(A5),DAY(A5))</f>
+        <v>44910</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B9" ca="1" si="0">(A6-$B$1)/360</f>
+        <v>1.1916666666666667</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D9" ca="1" si="1">EXP(-$B$2*B6)</f>
+        <v>0.87714467595565471</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E9" ca="1" si="2">C6*D6</f>
+        <v>87.714467595565466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f t="shared" ref="A7:A9" si="3">DATE(YEAR(A6)+1,MONTH(A6),DAY(A6))</f>
+        <v>45275</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2055555555555557</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78457656756130434</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="2"/>
+        <v>78.457656756130433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="3"/>
+        <v>45641</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2222222222222223</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70156309223617408</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="2"/>
+        <v>70.156309223617413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="3"/>
+        <v>46006</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2361111111111107</v>
+      </c>
+      <c r="C9">
+        <v>1100</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6275247150473271</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="2"/>
+        <v>690.27718655205979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5">
+        <f ca="1">SUM(E5:E9)</f>
+        <v>1024.6690615259379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796F6177-E793-4660-9E13-98734857215D}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
+        <f ca="1">TODAY()</f>
+        <v>44483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44561</v>
+      </c>
+      <c r="B5">
+        <f ca="1">(A5-$B$1)/360</f>
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <f ca="1">EXP(-$B$2*B5)</f>
+        <v>0.97644843760314604</v>
+      </c>
+      <c r="E5">
+        <f ca="1">C5*D5</f>
+        <v>97.6448437603146</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -502,19 +675,19 @@
         <v>44926</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B9" ca="1" si="0">(A6-$B$1)/360</f>
-        <v>1.2361111111111112</v>
+        <f t="shared" ref="B6:B8" ca="1" si="0">(A6-$B$1)/360</f>
+        <v>1.2305555555555556</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D9" ca="1" si="1">EXP(-$B$2*B6)</f>
-        <v>0.87286687845414757</v>
+        <v>0.87340046012432959</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E9" ca="1" si="2">C6*D6</f>
-        <v>87.286687845414761</v>
+        <v>87.340046012432964</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -524,18 +697,18 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
+        <v>2.2444444444444445</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78075022081092571</v>
+        <v>0.78122749176380357</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
-        <v>78.07502208109257</v>
+        <v>78.122749176380353</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,18 +718,18 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2666666666666666</v>
+        <v>3.2611111111111111</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6981415986953875</v>
+        <v>0.69856837117289883</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>69.814159869538756</v>
+        <v>69.856837117289885</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,28 +738,25 @@
         <v>46022</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.2805555555555559</v>
+        <f ca="1">(A9-$B$1)/360</f>
+        <v>4.2750000000000004</v>
       </c>
       <c r="C9">
         <v>1100</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62446430354196303</v>
+        <v>0.6248460372453235</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>686.91073389615929</v>
+        <v>687.33064096985584</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="E10" s="4">
         <f ca="1">SUM(E5:E9)</f>
-        <v>1019.6717938329067</v>
+        <v>1020.2951170362737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>